<commit_message>
Update API Security Concerns Excel files
- Updated the API Security Concerns rating and effectiveness Excel files to incorporate the latest data and insights on security risks and current solutions.
</commit_message>
<xml_diff>
--- a/data/Section 3/3.0 Overall/8 API Security Concerns- Rating.xlsx
+++ b/data/Section 3/3.0 Overall/8 API Security Concerns- Rating.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://netorgft15392477-my.sharepoint.com/personal/nitin_acharekar_smartvalyou_ai/Documents/Survey Report/Survey Report Agent/surveyreport/data/Section 3/3.0 Overall/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="25" documentId="8_{8A732019-FF50-45B6-832A-E1CB60AB97D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2A9354D0-DB7E-44A5-A8DC-E84AD473A3D3}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="8_{8A732019-FF50-45B6-832A-E1CB60AB97D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D17B6B7D-8C77-486D-AA61-1A4FF59EA120}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{3F0DFBEF-9761-4397-AAC7-783AECD8A846}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3F0DFBEF-9761-4397-AAC7-783AECD8A846}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="Legend" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -588,7 +588,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2824282A-1E00-4383-9BF7-9C210F636414}">
   <dimension ref="A1:K1001"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
@@ -35643,7 +35643,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4781B72-92C1-4E05-820F-A0D64DD87D62}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -35726,6 +35726,14 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="dc48c5df-3b0f-414f-aba8-6581fa801985" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010052F5D8B0E75D644F9CCB713FEA75AA22" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="49a44777f8da62b572afdb6b2055cc96">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="dc48c5df-3b0f-414f-aba8-6581fa801985" xmlns:ns4="7c288d03-abb0-40cb-a891-02024b2e663f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="109f530913ca07441dc83e0537539bfd" ns3:_="" ns4:_="">
     <xsd:import namespace="dc48c5df-3b0f-414f-aba8-6581fa801985"/>
@@ -35958,14 +35966,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="dc48c5df-3b0f-414f-aba8-6581fa801985" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A5EA7C5A-7559-402D-AAB8-B283B0EC6D20}">
   <ds:schemaRefs>
@@ -35975,6 +35975,23 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1291BD34-CB4E-4EB0-80CF-B1F463FCEBF7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="dc48c5df-3b0f-414f-aba8-6581fa801985"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="7c288d03-abb0-40cb-a891-02024b2e663f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{261D4D4D-5706-4D96-BB0A-F568A3B33E14}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -35991,21 +36008,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1291BD34-CB4E-4EB0-80CF-B1F463FCEBF7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="dc48c5df-3b0f-414f-aba8-6581fa801985"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="7c288d03-abb0-40cb-a891-02024b2e663f"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>